<commit_message>
Minor amends in pfscompd
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/maic_app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/maic_tutorial/maic_tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C404F64-E4AD-6542-BB21-83308C2E020F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C1C8F1-1128-4D4B-BA04-76A53E277CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="900" windowWidth="25040" windowHeight="14180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="760" windowWidth="25040" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pfsipd" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="10">
   <si>
     <t>TRT</t>
   </si>
@@ -13155,10 +13155,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8478E2A6-4C7C-ED40-B094-8057CEE0FFCA}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13597,7 +13597,7 @@
         <v>4.1027777708333328</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -13608,9 +13608,207 @@
         <v>4.7347222152777775</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>5.3666666597222203</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>5.9986111041666597</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>6.6305555486111096</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>7.2624999930555498</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>7.8944444374999998</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>8.52638888194444</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>9.15833332638889</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>9.7902777708333293</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>10.422222215277801</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>11.054166659722201</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>11.686111104166701</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>12.318055548611101</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>12.9499999930556</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>13.581944437500001</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>14.213888881944399</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>14.845833326388901</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>15.477777770833301</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>16.109722215277699</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
         <v>9</v>
       </c>
     </row>
@@ -13623,7 +13821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC4A4C25-B45E-0046-BE7D-C7CEF2666D7F}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>